<commit_message>
Got Ablock test working well
</commit_message>
<xml_diff>
--- a/Prototypes/SCUM/CropCoeff.xlsx
+++ b/Prototypes/SCUM/CropCoeff.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="29715" windowHeight="20745" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="6" r:id="rId1"/>
     <sheet name="CoreParams" sheetId="5" r:id="rId2"/>
     <sheet name="AllParams" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterate="1"/>
 </workbook>
 </file>
 
@@ -4926,23 +4926,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="133045632"/>
-        <c:axId val="133076096"/>
+        <c:axId val="48694784"/>
+        <c:axId val="48696320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133045632"/>
+        <c:axId val="48694784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133076096"/>
+        <c:crossAx val="48696320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133076096"/>
+        <c:axId val="48696320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4950,7 +4950,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133045632"/>
+        <c:crossAx val="48694784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4962,7 +4962,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10351,7 +10351,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="5">
-        <f t="shared" ref="B35:B66" si="16">X35-C35</f>
+        <f t="shared" ref="B35:B52" si="16">X35-C35</f>
         <v>563</v>
       </c>
       <c r="C35" s="5">
@@ -10435,7 +10435,7 @@
         <v>9.9330714907571532E-2</v>
       </c>
       <c r="AC35" s="5">
-        <f t="shared" ref="AC35:AC66" si="17">(AA35-AB35)*(H35)</f>
+        <f t="shared" ref="AC35:AC52" si="17">(AA35-AB35)*(H35)</f>
         <v>9.3867525587655085E-2</v>
       </c>
       <c r="AD35" s="5">
@@ -13115,10 +13115,10 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14320,7 +14320,7 @@
         <v>0.45</v>
       </c>
       <c r="F22">
-        <v>700</v>
+        <v>1200</v>
       </c>
       <c r="G22">
         <v>0.1</v>
@@ -14376,7 +14376,7 @@
         <v>0.5</v>
       </c>
       <c r="F23">
-        <v>700</v>
+        <v>1200</v>
       </c>
       <c r="G23">
         <v>0.1</v>
@@ -14488,7 +14488,7 @@
         <v>0.89300000000000002</v>
       </c>
       <c r="F25">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="G25">
         <v>0.1</v>
@@ -14544,7 +14544,7 @@
         <v>0.90399999999999991</v>
       </c>
       <c r="F26">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="G26">
         <v>0.1</v>
@@ -14600,7 +14600,7 @@
         <v>0.91099999999999992</v>
       </c>
       <c r="F27">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="G27">
         <v>0.1</v>

</xml_diff>